<commit_message>
Added equal temperament scale, and gave chord definitions.
</commit_message>
<xml_diff>
--- a/Project 1/hw1_table.xlsx
+++ b/Project 1/hw1_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nivelnola\Documents\Cooper Union Files\Y3-S2\ECE-413 Music &amp; Engineering\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF2DFC6-3C12-4EA7-943C-59F6A700DE79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD28342-183C-4449-B569-FAA1A785F754}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -122,7 +122,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -258,32 +258,32 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -629,8 +629,8 @@
   </sheetPr>
   <dimension ref="A1:XFD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,24 +639,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16 16384:16384" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
     </row>
     <row r="2" spans="1:16 16384:16384" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -750,7 +750,7 @@
       <c r="F4" s="2">
         <v>220</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="11">
         <v>220</v>
       </c>
       <c r="H4" s="2">
@@ -925,7 +925,7 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="15">
+      <c r="D11" s="10">
         <f>G4*3/2</f>
         <v>330</v>
       </c>
@@ -1038,24 +1038,24 @@
       <c r="P15" s="3"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -1112,23 +1112,23 @@
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="17">
         <v>440</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="19"/>
       <c r="R19" s="6"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
@@ -1421,6 +1421,11 @@
     <row r="48" ht="29.55" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A17:P17"/>
+    <mergeCell ref="B19:P19"/>
+    <mergeCell ref="B20:P20"/>
+    <mergeCell ref="B21:P21"/>
     <mergeCell ref="B27:P27"/>
     <mergeCell ref="B28:P28"/>
     <mergeCell ref="B29:P29"/>
@@ -1430,11 +1435,6 @@
     <mergeCell ref="B24:P24"/>
     <mergeCell ref="B25:P25"/>
     <mergeCell ref="B26:P26"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A17:P17"/>
-    <mergeCell ref="B19:P19"/>
-    <mergeCell ref="B20:P20"/>
-    <mergeCell ref="B21:P21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
All sounds work, Just table filled in w/ major scales
</commit_message>
<xml_diff>
--- a/Project 1/hw1_table.xlsx
+++ b/Project 1/hw1_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nivelnola\Documents\Cooper Union Files\Y3-S2\ECE-413 Music &amp; Engineering\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCF675F-EFB6-4D5C-BAC5-D60B1617CBAC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269DDB5F-5DDE-46F5-B221-E7A32089754B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -711,13 +711,12 @@
   <dimension ref="A1:AI56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="20820" topLeftCell="Y1"/>
-      <selection activeCell="B2" sqref="B2"/>
-      <selection pane="topRight" activeCell="Y3" sqref="Y3"/>
+      <selection activeCell="AI23" sqref="AI23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -848,23 +847,35 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="J3" s="2">
+        <f>J12*S12/2</f>
+        <v>412.5</v>
+      </c>
+      <c r="K3" s="2">
+        <f>K15*S9/2</f>
+        <v>417.18518518518522</v>
+      </c>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="M3" s="2">
+        <f>M21*S6/2</f>
+        <v>412.5</v>
+      </c>
       <c r="N3" s="9">
         <f>(B4/S4)</f>
         <v>412.5</v>
       </c>
       <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="P3" s="2">
+        <f>P9*S14/2</f>
+        <v>419.04761904761904</v>
+      </c>
       <c r="R3" s="22" t="s">
         <v>33</v>
       </c>
       <c r="S3" s="23">
         <v>1</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="22" t="s">
         <v>51</v>
       </c>
       <c r="U3" t="s">
@@ -941,6 +952,7 @@
         <f>16/15</f>
         <v>1.0666666666666667</v>
       </c>
+      <c r="T4" s="22"/>
       <c r="AG4" s="22" t="s">
         <v>5</v>
       </c>
@@ -958,8 +970,14 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="2">
+        <f>H7*S18/2</f>
+        <v>458.33333333333331</v>
+      </c>
+      <c r="I5" s="2">
+        <f>I11*S14/2</f>
+        <v>458.33333333333337</v>
+      </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -977,6 +995,7 @@
         <f>10/9</f>
         <v>1.1111111111111112</v>
       </c>
+      <c r="T5" s="22"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -990,13 +1009,31 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="J6" s="2">
+        <f>J12*S14/2</f>
+        <v>458.33333333333337</v>
+      </c>
+      <c r="K6" s="2">
+        <f>K15*S12/2</f>
+        <v>469.33333333333337</v>
+      </c>
+      <c r="L6" s="2">
+        <f>L19*S9/2</f>
+        <v>469.33333333333331</v>
+      </c>
+      <c r="M6" s="2">
+        <f>M21*S8/2</f>
+        <v>458.33333333333337</v>
+      </c>
+      <c r="N6" s="2">
+        <f>N3*S6</f>
+        <v>464.0625</v>
+      </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="P6" s="2">
+        <f>P9*S18/2</f>
+        <v>471.42857142857139</v>
+      </c>
       <c r="R6" s="22" t="s">
         <v>36</v>
       </c>
@@ -1004,7 +1041,7 @@
         <f>9/8</f>
         <v>1.125</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="22" t="s">
         <v>52</v>
       </c>
       <c r="U6" t="s">
@@ -1077,7 +1114,10 @@
         <f>F22*S8/2</f>
         <v>488.88888888888886</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2">
+        <f>B4*S6</f>
+        <v>495</v>
+      </c>
       <c r="H7" s="9">
         <f>(B4/S17)*2</f>
         <v>488.88888888888886</v>
@@ -1097,6 +1137,7 @@
         <f>6/5</f>
         <v>1.2</v>
       </c>
+      <c r="T7" s="22"/>
       <c r="X7" s="22" t="s">
         <v>5</v>
       </c>
@@ -1115,7 +1156,10 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="I8" s="2">
+        <f>I11*S18/2</f>
+        <v>515.625</v>
+      </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1130,7 +1174,7 @@
         <f>5/4</f>
         <v>1.25</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="22" t="s">
         <v>53</v>
       </c>
       <c r="U8" t="s">
@@ -1194,7 +1238,10 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
+      <c r="M9" s="2">
+        <f>M21*S9/2</f>
+        <v>488.88888888888891</v>
+      </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="9">
@@ -1208,7 +1255,7 @@
         <f>4/3</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="22" t="s">
         <v>50</v>
       </c>
       <c r="U9" t="s">
@@ -1275,12 +1322,27 @@
       <c r="G10" s="2"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="J10" s="3">
+        <f>J12*S18/2</f>
+        <v>515.625</v>
+      </c>
+      <c r="K10" s="3">
+        <f>K15*S14/2</f>
+        <v>521.48148148148152</v>
+      </c>
+      <c r="L10" s="3">
+        <f>L19*S12/2</f>
+        <v>528</v>
+      </c>
       <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="N10" s="3">
+        <f>N3*S8</f>
+        <v>515.625</v>
+      </c>
+      <c r="O10" s="3">
+        <f>O5*S6</f>
+        <v>528</v>
+      </c>
       <c r="P10" s="3"/>
       <c r="R10" t="s">
         <v>40</v>
@@ -1289,6 +1351,7 @@
         <f>45/32</f>
         <v>1.40625</v>
       </c>
+      <c r="T10" s="22"/>
       <c r="AD10" s="22" t="s">
         <v>5</v>
       </c>
@@ -1311,8 +1374,14 @@
         <v>550</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="2">
+        <f>B4*S8</f>
+        <v>550</v>
+      </c>
+      <c r="H11" s="3">
+        <f>H7*S6</f>
+        <v>550</v>
+      </c>
       <c r="I11" s="9">
         <f>(B4/S13)*2</f>
         <v>550</v>
@@ -1330,6 +1399,7 @@
         <f>64/45</f>
         <v>1.4222222222222223</v>
       </c>
+      <c r="T11" s="22"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1349,10 +1419,19 @@
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+      <c r="M12" s="3">
+        <f>M21*S12/2</f>
+        <v>550</v>
+      </c>
+      <c r="N12" s="3">
+        <f>N3*S9</f>
+        <v>550</v>
+      </c>
       <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
+      <c r="P12" s="3">
+        <f>P9*S6</f>
+        <v>565.71428571428567</v>
+      </c>
       <c r="R12" s="22" t="s">
         <v>42</v>
       </c>
@@ -1360,7 +1439,7 @@
         <f>3/2</f>
         <v>1.5</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="22" t="s">
         <v>52</v>
       </c>
       <c r="U12" t="s">
@@ -1427,15 +1506,27 @@
         <f>F22*S12/2</f>
         <v>586.66666666666663</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2">
+        <f>B4*S9</f>
+        <v>586.66666666666663</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="K13" s="3">
+        <f>K15*S18/2</f>
+        <v>586.66666666666674</v>
+      </c>
+      <c r="L13" s="3">
+        <f>L19*S14/2</f>
+        <v>586.66666666666674</v>
+      </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="O13" s="3">
+        <f>O5*S8</f>
+        <v>586.66666666666663</v>
+      </c>
       <c r="P13" s="3"/>
       <c r="R13" t="s">
         <v>43</v>
@@ -1444,6 +1535,7 @@
         <f>8/5</f>
         <v>1.6</v>
       </c>
+      <c r="T13" s="22"/>
       <c r="AB13" s="22" t="s">
         <v>5</v>
       </c>
@@ -1467,8 +1559,14 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="H14" s="3">
+        <f>H7*S8</f>
+        <v>611.11111111111109</v>
+      </c>
+      <c r="I14" s="3">
+        <f>I11*S6</f>
+        <v>618.75</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1483,7 +1581,7 @@
         <f>5/3</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="22" t="s">
         <v>53</v>
       </c>
       <c r="U14" s="22" t="s">
@@ -1544,16 +1642,31 @@
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="J15" s="3">
+        <f>J12*S6</f>
+        <v>618.75</v>
+      </c>
       <c r="K15" s="9">
         <f>(B4/S10)*2</f>
         <v>625.77777777777783</v>
       </c>
       <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
+      <c r="M15" s="3">
+        <f>M21*S14/2</f>
+        <v>611.1111111111112</v>
+      </c>
+      <c r="N15" s="3">
+        <f>N3*S12</f>
+        <v>618.75</v>
+      </c>
+      <c r="O15" s="3">
+        <f>O5*S9</f>
+        <v>625.77777777777771</v>
+      </c>
+      <c r="P15" s="3">
+        <f>P9*S8</f>
+        <v>628.57142857142856</v>
+      </c>
       <c r="R15" t="s">
         <v>45</v>
       </c>
@@ -1561,6 +1674,7 @@
         <f>7/4</f>
         <v>1.75</v>
       </c>
+      <c r="T15" s="22"/>
       <c r="AI15" s="22" t="s">
         <v>5</v>
       </c>
@@ -1586,12 +1700,21 @@
         <f>F22*S14/2</f>
         <v>651.85185185185185</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
+      <c r="G16" s="2">
+        <f>B4*S12</f>
+        <v>660</v>
+      </c>
+      <c r="H16" s="3">
+        <f>H7*S9</f>
+        <v>651.85185185185173</v>
+      </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="L16" s="3">
+        <f>L19*S18/2</f>
+        <v>660</v>
+      </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
@@ -1603,6 +1726,7 @@
         <f>16/9</f>
         <v>1.7777777777777777</v>
       </c>
+      <c r="T16" s="22"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -1618,7 +1742,10 @@
       <c r="F17" s="3"/>
       <c r="G17" s="2"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3">
+        <f>I11*S8</f>
+        <v>687.5</v>
+      </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1633,6 +1760,7 @@
         <f>9/5</f>
         <v>1.8</v>
       </c>
+      <c r="T17" s="22"/>
       <c r="AA17" s="22" t="s">
         <v>5</v>
       </c>
@@ -1655,7 +1783,10 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
+      <c r="P18" s="3">
+        <f>P9*S9</f>
+        <v>670.47619047619037</v>
+      </c>
       <c r="R18" s="22" t="s">
         <v>48</v>
       </c>
@@ -1663,7 +1794,7 @@
         <f>15/8</f>
         <v>1.875</v>
       </c>
-      <c r="T18" t="s">
+      <c r="T18" s="22" t="s">
         <v>52</v>
       </c>
       <c r="U18" t="s">
@@ -1727,15 +1858,30 @@
       <c r="G19" s="2"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="J19" s="3">
+        <f>J12*S8</f>
+        <v>687.5</v>
+      </c>
+      <c r="K19" s="3">
+        <f>K15*S6</f>
+        <v>704</v>
+      </c>
       <c r="L19" s="9">
         <f>(B4/S8)*2</f>
         <v>704</v>
       </c>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
+      <c r="M19" s="3">
+        <f>M21*S18/2</f>
+        <v>687.5</v>
+      </c>
+      <c r="N19" s="3">
+        <f>N3*S14</f>
+        <v>687.5</v>
+      </c>
+      <c r="O19" s="3">
+        <f>O5*S12</f>
+        <v>704</v>
+      </c>
       <c r="P19" s="3"/>
       <c r="R19" s="22" t="s">
         <v>49</v>
@@ -1743,7 +1889,7 @@
       <c r="S19" s="23">
         <v>2</v>
       </c>
-      <c r="T19" t="s">
+      <c r="T19" s="22" t="s">
         <v>50</v>
       </c>
       <c r="U19" t="s">
@@ -1762,7 +1908,7 @@
         <v>4</v>
       </c>
       <c r="Z19" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="AA19" t="s">
         <v>6</v>
@@ -1813,9 +1959,18 @@
         <f>F22*S18/2</f>
         <v>733.33333333333326</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="G20" s="3">
+        <f>B4*S14</f>
+        <v>733.33333333333337</v>
+      </c>
+      <c r="H20" s="3">
+        <f>H7*S12</f>
+        <v>733.33333333333326</v>
+      </c>
+      <c r="I20" s="3">
+        <f>I11*S9</f>
+        <v>733.33333333333326</v>
+      </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1836,7 +1991,10 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="J21" s="3">
+        <f>J12*S9</f>
+        <v>733.33333333333326</v>
+      </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="9">
@@ -1845,7 +2003,10 @@
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
+      <c r="P21" s="3">
+        <f>P9*S12</f>
+        <v>754.28571428571422</v>
+      </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1869,11 +2030,23 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="K22" s="3">
+        <f>K15*S8</f>
+        <v>782.22222222222229</v>
+      </c>
+      <c r="L22" s="3">
+        <f>L19*S6</f>
+        <v>792</v>
+      </c>
       <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
+      <c r="N22" s="3">
+        <f>N3*S18</f>
+        <v>773.4375</v>
+      </c>
+      <c r="O22" s="3">
+        <f>O5*S14</f>
+        <v>782.22222222222217</v>
+      </c>
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
@@ -1891,9 +2064,18 @@
         <v>825</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="G23" s="3">
+        <f>B4*S18</f>
+        <v>825</v>
+      </c>
+      <c r="H23" s="3">
+        <f>H7*S14</f>
+        <v>814.81481481481478</v>
+      </c>
+      <c r="I23" s="3">
+        <f>I11*S12</f>
+        <v>825</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>

</xml_diff>